<commit_message>
Go back to old BusinessOwners.xlsx
Newer one only had 100 features. Older one had 171. Going back to old one so we don't have to update a tonne of screen captures.
</commit_message>
<xml_diff>
--- a/Data/Planning/BusinessOwners.xlsx
+++ b/Data/Planning/BusinessOwners.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="392">
   <si>
     <t>Last Name</t>
   </si>
@@ -1192,6 +1192,9 @@
   </si>
   <si>
     <t>B6E3D0</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -1655,10 +1658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:F172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102:XFD177"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3690,6 +3693,361 @@
         <v>49.280655622540003</v>
       </c>
     </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D105" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D108" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D109" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D110" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D111" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D112" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D113" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D114" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D115" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D116" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D117" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D118" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D119" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D120" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D121" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D122" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D123" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D124" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D125" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D126" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D127" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D128" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D129" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D130" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D131" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D132" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D133" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D134" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D135" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D136" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D137" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D138" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D139" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D140" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D141" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="142" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D142" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="143" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D143" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="144" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D144" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D145" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D146" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D147" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D148" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D149" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D150" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D151" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D152" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D153" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D154" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="155" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D155" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D156" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="157" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D157" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="158" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D158" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="159" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D159" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="160" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D160" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="161" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D161" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="162" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D162" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="163" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D163" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="164" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D164" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="165" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D165" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="166" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D166" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="167" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D167" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="168" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D168" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="169" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D169" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="170" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D170" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="171" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D171" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="172" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D172" t="s">
+        <v>391</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>